<commit_message>
EPICP-1 updates to DPE from Tracy (including the changed algorithm from Flo for education)
</commit_message>
<xml_diff>
--- a/analyst/Tracy/rmonize/data_proc_elem/DPE_EPICP_TRACY.xlsx
+++ b/analyst/Tracy/rmonize/data_proc_elem/DPE_EPICP_TRACY.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Projekte\NFDI4Health\TA5\Pilotprojekte\Harmonisierung\HarmonizR\use-cases-harmonisation\analyst\Tracy\rmonize\data_proc_elem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54207243-7CF8-4C61-8037-5E656658FF05}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F1D4D12-BA5C-465C-BCEA-02A87349F120}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="12" windowWidth="16092" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -491,9 +491,6 @@
     <t>id_creation</t>
   </si>
   <si>
-    <t>recode(0=3; 1=0; 1=2; 2=1; 9="")</t>
-  </si>
-  <si>
     <t>partial</t>
   </si>
   <si>
@@ -514,9 +511,6 @@
 1= alive;
 2= dead;
 6=dropped out</t>
-  </si>
-  <si>
-    <t>recode(1 = 3; 2= 5; 3= 5; 4= 3; 5= 2; 6= 4; 7= 4)</t>
   </si>
   <si>
     <r>
@@ -589,9 +583,6 @@
     <t>age0</t>
   </si>
   <si>
-    <t>educc7</t>
-  </si>
-  <si>
     <t>PAL</t>
   </si>
   <si>
@@ -685,12 +676,6 @@
     </r>
   </si>
   <si>
-    <t>case_when(
-casestroke_fup5 == 0 ~ 0;
-casestroke_fup5 == 2 ~ 1;
-casestroke_fup5 == 6 ~ 1)</t>
-  </si>
-  <si>
     <r>
       <t>age0 + ((</t>
     </r>
@@ -715,12 +700,6 @@
     </r>
   </si>
   <si>
-    <t>case_when(
-casemi_fup5 == 0 ~ 0;
-casemi_fup5 == 2 ~ 1;
-casemi_fup5 == 5 ~ 1)</t>
-  </si>
-  <si>
     <r>
       <t>age0 + ((</t>
     </r>
@@ -745,11 +724,6 @@
     </r>
   </si>
   <si>
-    <t>case_when(
-casehf_fup5 == 0 ~ 0;
-casehf_fup5 == 2 ~ 1)</t>
-  </si>
-  <si>
     <t xml:space="preserve">complete </t>
   </si>
   <si>
@@ -771,11 +745,6 @@
     </r>
   </si>
   <si>
-    <t>case_when(
-casediab_fup5 == 0 ~ 0;
-casediab_fup5 == 2 ~ 1)</t>
-  </si>
-  <si>
     <t>age0 + ((dd_incdiab - DAT_REKR)/365.25)</t>
   </si>
   <si>
@@ -783,17 +752,6 @@
   </si>
   <si>
     <t>number of children minus stillbirths</t>
-  </si>
-  <si>
-    <t>case_when(
-casemi_fup5 == 0 | casestroke_fup5 == 0 | casehf_fup5 == 0 ~ 0;
-casemi_fup5 == 2 | casestroke_fup5 == 2 | casehf_fup5 == 2 ~ 1;
-casemi_fup5 == 5 | casestroke_fup5 == 6 ~ 1)</t>
-  </si>
-  <si>
-    <t>case_when(
-casehyp_fup5 == 0 ~ 0;
-casehyp_fup5 == 2 ~ 1)</t>
   </si>
   <si>
     <r>
@@ -919,15 +877,7 @@
     <t>first occuring tumor (derived from ICDO2 or ICDO3 code); yes/no coded</t>
   </si>
   <si>
-    <t>prim_canc_fup5</t>
-  </si>
-  <si>
     <t>prevmi;prevstroke</t>
-  </si>
-  <si>
-    <t>case_when(
-prevmi == 0 | prevstroke == 0  ~ 0;
-prevmi == 1 | prevstroke == 1 ~ 1;</t>
   </si>
   <si>
     <t>age0 + (ysmkces0- format(as.Date(DAT_REKR, format="%d/%m/%Y"),"%Y")</t>
@@ -962,6 +912,66 @@
       </rPr>
       <t>ysmkces0</t>
     </r>
+  </si>
+  <si>
+    <t>inccanc_fup5</t>
+  </si>
+  <si>
+    <t>recode(0=3; 1=0; 1=2; 2=1; 9=NA)</t>
+  </si>
+  <si>
+    <t>case_when(
+prevmi == 0 | prevstroke == 0  ~ 0L,
+prevmi == 1 | prevstroke == 1 ~ 1L, 
+TRUE ~ NA_integer_)</t>
+  </si>
+  <si>
+    <t>case_when(
+casemi_fup5 %in% c(0) | casestroke_fup5 %in% c(0) | casehf_fup5 %in% c(0) ~ 0L,
+casemi_fup5 %in% c(2,5) | casestroke_fup5 %in% c(2,6) | casehf_fup5 == 2 ~ 1L, TRUE ~ NA_integer_)</t>
+  </si>
+  <si>
+    <t>case_when(
+casemi_fup5 %in% c(0) ~ 0L,
+casemi_fup5 %in% c(2,5) ~ 1L,
+TRUE ~ NA_integer_))</t>
+  </si>
+  <si>
+    <t>case_when(
+casestroke_fup5 %in% c(0) ~ 0L,
+casestroke_fup5 %in% c(2,6) ~ 1L,
+TRUE ~ NA_integer_)</t>
+  </si>
+  <si>
+    <t>case_when(
+casehyp_fup5 == 0 ~ 0L,
+casehyp_fup5 == 2 ~ 1L,
+TRUE ~ NA_integer_)</t>
+  </si>
+  <si>
+    <t>case_when(
+casehf_fup5 == 0 ~ 0L,
+casehf_fup5 == 2 ~ 1L,
+TRUE ~ NA_integer_)</t>
+  </si>
+  <si>
+    <t>case_when(
+casediab_fup5 == 0 ~ 0L,
+casediab_fup5 == 2 ~ 1L,
+TRUE ~ NA_integer_)</t>
+  </si>
+  <si>
+    <t>case_when(
+educc7 %in% c(7) ~ 7L,
+educc7 %in% c(5,6) ~ 6L,
+educc7 %in% c(3,4) ~ 4L,
+abschlus %in% c(3,4) ~ 3L,
+abschlus %in% c(1,2) ~ 2L,
+abschlus %in% c(5) ~ 0L,
+TRUE ~ NA_integer_)</t>
+  </si>
+  <si>
+    <t>educc7;abschlus</t>
   </si>
 </sst>
 </file>
@@ -1048,9 +1058,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1074,6 +1081,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1415,24 +1425,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" topLeftCell="B43" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="H58" sqref="H58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="46.5546875" customWidth="1"/>
-    <col min="5" max="5" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="46.5703125" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="66.109375" customWidth="1"/>
-    <col min="9" max="9" width="54.5546875" customWidth="1"/>
-    <col min="10" max="10" width="18.109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="23.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="73.85546875" customWidth="1"/>
+    <col min="9" max="9" width="54.5703125" customWidth="1"/>
+    <col min="10" max="10" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="23.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1467,7 +1477,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>11</v>
       </c>
@@ -1493,7 +1503,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>14</v>
       </c>
@@ -1504,7 +1514,7 @@
         <v>13</v>
       </c>
       <c r="F3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="G3" t="s">
         <v>149</v>
@@ -1519,7 +1529,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>16</v>
       </c>
@@ -1530,7 +1540,7 @@
         <v>18</v>
       </c>
       <c r="F4" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="G4" t="s">
         <v>149</v>
@@ -1545,7 +1555,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>19</v>
       </c>
@@ -1556,13 +1566,13 @@
         <v>13</v>
       </c>
       <c r="F5" t="s">
-        <v>169</v>
+        <v>220</v>
       </c>
       <c r="G5" t="s">
         <v>150</v>
       </c>
-      <c r="H5" s="7" t="s">
-        <v>162</v>
+      <c r="H5" s="17" t="s">
+        <v>219</v>
       </c>
       <c r="J5" t="s">
         <v>151</v>
@@ -1571,7 +1581,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>21</v>
       </c>
@@ -1582,7 +1592,7 @@
         <v>18</v>
       </c>
       <c r="F6" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="G6" t="s">
         <v>149</v>
@@ -1597,7 +1607,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>23</v>
       </c>
@@ -1608,7 +1618,7 @@
         <v>13</v>
       </c>
       <c r="F7" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="G7" t="s">
         <v>149</v>
@@ -1623,7 +1633,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>25</v>
       </c>
@@ -1634,13 +1644,13 @@
         <v>13</v>
       </c>
       <c r="F8" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="G8" t="s">
         <v>150</v>
       </c>
-      <c r="H8" s="16" t="s">
-        <v>188</v>
+      <c r="H8" s="15" t="s">
+        <v>185</v>
       </c>
       <c r="J8" t="s">
         <v>151</v>
@@ -1649,7 +1659,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>27</v>
       </c>
@@ -1675,7 +1685,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>29</v>
       </c>
@@ -1701,7 +1711,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>31</v>
       </c>
@@ -1727,7 +1737,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>33</v>
       </c>
@@ -1738,13 +1748,13 @@
         <v>18</v>
       </c>
       <c r="F12" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>154</v>
       </c>
       <c r="H12" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="J12" s="2" t="s">
         <v>151</v>
@@ -1753,7 +1763,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>35</v>
       </c>
@@ -1763,14 +1773,14 @@
       <c r="D13" t="s">
         <v>18</v>
       </c>
-      <c r="F13" s="17" t="s">
-        <v>220</v>
+      <c r="F13" s="16" t="s">
+        <v>209</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="H13" s="16" t="s">
-        <v>219</v>
+      <c r="H13" s="15" t="s">
+        <v>208</v>
       </c>
       <c r="J13" s="2" t="s">
         <v>151</v>
@@ -1779,7 +1789,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>37</v>
       </c>
@@ -1790,7 +1800,7 @@
         <v>13</v>
       </c>
       <c r="F14" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>149</v>
@@ -1805,7 +1815,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="72" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>39</v>
       </c>
@@ -1816,25 +1826,25 @@
         <v>13</v>
       </c>
       <c r="F15" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>150</v>
       </c>
       <c r="H15" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="I15" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="J15" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="I15" s="8" t="s">
-        <v>158</v>
-      </c>
-      <c r="J15" s="2" t="s">
-        <v>157</v>
-      </c>
       <c r="K15" s="2" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>41</v>
       </c>
@@ -1845,7 +1855,7 @@
         <v>13</v>
       </c>
       <c r="F16" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="G16" s="2" t="s">
         <v>149</v>
@@ -1860,7 +1870,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>43</v>
       </c>
@@ -1871,7 +1881,7 @@
         <v>13</v>
       </c>
       <c r="F17" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="G17" s="2" t="s">
         <v>149</v>
@@ -1886,7 +1896,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>45</v>
       </c>
@@ -1897,16 +1907,16 @@
         <v>13</v>
       </c>
       <c r="F18" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="G18" t="s">
         <v>154</v>
       </c>
       <c r="H18" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="I18" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="J18" t="s">
         <v>151</v>
@@ -1915,7 +1925,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>47</v>
       </c>
@@ -1926,7 +1936,7 @@
         <v>18</v>
       </c>
       <c r="F19" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="G19" t="s">
         <v>149</v>
@@ -1941,7 +1951,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>49</v>
       </c>
@@ -1967,7 +1977,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>51</v>
       </c>
@@ -1993,7 +2003,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="22" spans="2:11" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:11" ht="60" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>53</v>
       </c>
@@ -2004,13 +2014,13 @@
         <v>13</v>
       </c>
       <c r="F22" t="s">
-        <v>217</v>
+        <v>207</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="H22" s="13" t="s">
-        <v>218</v>
+        <v>158</v>
+      </c>
+      <c r="H22" s="12" t="s">
+        <v>212</v>
       </c>
       <c r="J22" t="s">
         <v>151</v>
@@ -2019,7 +2029,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>55</v>
       </c>
@@ -2045,7 +2055,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>57</v>
       </c>
@@ -2071,7 +2081,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>59</v>
       </c>
@@ -2097,7 +2107,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>61</v>
       </c>
@@ -2123,7 +2133,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>63</v>
       </c>
@@ -2149,7 +2159,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="28" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>65</v>
       </c>
@@ -2175,7 +2185,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="29" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>67</v>
       </c>
@@ -2201,7 +2211,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="30" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>69</v>
       </c>
@@ -2227,7 +2237,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="31" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>71</v>
       </c>
@@ -2253,7 +2263,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="32" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>73</v>
       </c>
@@ -2279,7 +2289,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="33" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>75</v>
       </c>
@@ -2305,7 +2315,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="34" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>77</v>
       </c>
@@ -2316,7 +2326,7 @@
         <v>13</v>
       </c>
       <c r="F34" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="G34" s="2" t="s">
         <v>149</v>
@@ -2331,7 +2341,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="35" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>79</v>
       </c>
@@ -2342,7 +2352,7 @@
         <v>13</v>
       </c>
       <c r="F35" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="G35" s="2" t="s">
         <v>149</v>
@@ -2357,7 +2367,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="36" spans="2:11" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:11" ht="90" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>81</v>
       </c>
@@ -2367,17 +2377,17 @@
       <c r="D36" t="s">
         <v>13</v>
       </c>
-      <c r="F36" s="14" t="s">
+      <c r="F36" s="13" t="s">
         <v>140</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="H36" s="13" t="s">
-        <v>205</v>
+        <v>158</v>
+      </c>
+      <c r="H36" s="12" t="s">
+        <v>213</v>
       </c>
       <c r="I36" s="5" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="J36" s="2" t="s">
         <v>151</v>
@@ -2386,7 +2396,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="37" spans="2:11" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:11" ht="45" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>83</v>
       </c>
@@ -2396,14 +2406,14 @@
       <c r="D37" t="s">
         <v>18</v>
       </c>
-      <c r="F37" s="14" t="s">
-        <v>181</v>
+      <c r="F37" s="13" t="s">
+        <v>178</v>
       </c>
       <c r="G37" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="H37" s="13" t="s">
-        <v>191</v>
+      <c r="H37" s="12" t="s">
+        <v>188</v>
       </c>
       <c r="J37" s="2" t="s">
         <v>151</v>
@@ -2412,7 +2422,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="38" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>85</v>
       </c>
@@ -2425,14 +2435,14 @@
       <c r="F38" t="s">
         <v>134</v>
       </c>
-      <c r="G38" s="9" t="s">
-        <v>135</v>
-      </c>
-      <c r="H38" s="9" t="s">
-        <v>135</v>
-      </c>
-      <c r="I38" s="10" t="s">
-        <v>210</v>
+      <c r="G38" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="H38" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="I38" s="9" t="s">
+        <v>201</v>
       </c>
       <c r="J38" s="2" t="s">
         <v>134</v>
@@ -2441,7 +2451,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="39" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>87</v>
       </c>
@@ -2454,13 +2464,13 @@
       <c r="F39" t="s">
         <v>134</v>
       </c>
-      <c r="G39" s="9" t="s">
-        <v>135</v>
-      </c>
-      <c r="H39" s="15" t="s">
-        <v>135</v>
-      </c>
-      <c r="I39" s="12"/>
+      <c r="G39" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="H39" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="I39" s="11"/>
       <c r="J39" s="2" t="s">
         <v>134</v>
       </c>
@@ -2468,7 +2478,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="40" spans="2:11" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:11" ht="60" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>89</v>
       </c>
@@ -2478,26 +2488,26 @@
       <c r="D40" t="s">
         <v>13</v>
       </c>
-      <c r="F40" s="15" t="s">
+      <c r="F40" s="14" t="s">
         <v>141</v>
       </c>
-      <c r="G40" s="9" t="s">
-        <v>159</v>
-      </c>
-      <c r="H40" s="14" t="s">
-        <v>195</v>
-      </c>
-      <c r="I40" s="10" t="s">
-        <v>209</v>
-      </c>
-      <c r="J40" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="K40" s="11" t="s">
+      <c r="G40" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="H40" s="13" t="s">
+        <v>214</v>
+      </c>
+      <c r="I40" s="9" t="s">
+        <v>200</v>
+      </c>
+      <c r="J40" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="K40" s="10" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="41" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>91</v>
       </c>
@@ -2508,23 +2518,23 @@
         <v>18</v>
       </c>
       <c r="F41" t="s">
-        <v>182</v>
-      </c>
-      <c r="G41" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="G41" s="8" t="s">
         <v>154</v>
       </c>
-      <c r="H41" s="9" t="s">
-        <v>192</v>
-      </c>
-      <c r="I41" s="12"/>
-      <c r="J41" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="K41" s="11" t="s">
+      <c r="H41" s="8" t="s">
+        <v>189</v>
+      </c>
+      <c r="I41" s="11"/>
+      <c r="J41" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="K41" s="10" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="42" spans="2:11" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:11" ht="60" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
         <v>93</v>
       </c>
@@ -2534,17 +2544,17 @@
       <c r="D42" t="s">
         <v>13</v>
       </c>
-      <c r="F42" s="15" t="s">
+      <c r="F42" s="14" t="s">
         <v>142</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="H42" s="13" t="s">
-        <v>193</v>
+        <v>158</v>
+      </c>
+      <c r="H42" s="12" t="s">
+        <v>215</v>
       </c>
       <c r="I42" s="5" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="J42" s="2" t="s">
         <v>151</v>
@@ -2553,7 +2563,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="43" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
         <v>95</v>
       </c>
@@ -2564,23 +2574,23 @@
         <v>18</v>
       </c>
       <c r="F43" t="s">
-        <v>183</v>
-      </c>
-      <c r="G43" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="G43" s="8" t="s">
         <v>154</v>
       </c>
-      <c r="H43" s="9" t="s">
-        <v>194</v>
-      </c>
-      <c r="I43" s="12"/>
-      <c r="J43" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="K43" s="11" t="s">
+      <c r="H43" s="8" t="s">
+        <v>190</v>
+      </c>
+      <c r="I43" s="11"/>
+      <c r="J43" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="K43" s="10" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="44" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
         <v>97</v>
       </c>
@@ -2590,26 +2600,26 @@
       <c r="D44" t="s">
         <v>13</v>
       </c>
-      <c r="F44" s="16" t="s">
+      <c r="F44" s="15" t="s">
         <v>143</v>
       </c>
-      <c r="G44" s="9" t="s">
+      <c r="G44" s="8" t="s">
         <v>149</v>
       </c>
       <c r="H44" t="s">
         <v>149</v>
       </c>
       <c r="I44" t="s">
-        <v>164</v>
-      </c>
-      <c r="J44" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="K44" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="J44" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="K44" s="10" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="45" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
         <v>99</v>
       </c>
@@ -2620,22 +2630,22 @@
         <v>18</v>
       </c>
       <c r="F45" t="s">
-        <v>183</v>
-      </c>
-      <c r="G45" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="G45" s="8" t="s">
         <v>154</v>
       </c>
-      <c r="H45" s="9" t="s">
-        <v>194</v>
-      </c>
-      <c r="J45" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="K45" s="11" t="s">
+      <c r="H45" s="8" t="s">
+        <v>190</v>
+      </c>
+      <c r="J45" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="K45" s="10" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="46" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
         <v>101</v>
       </c>
@@ -2645,23 +2655,23 @@
       <c r="D46" t="s">
         <v>13</v>
       </c>
-      <c r="F46" s="16" t="s">
+      <c r="F46" s="15" t="s">
         <v>144</v>
       </c>
-      <c r="G46" s="9" t="s">
+      <c r="G46" s="8" t="s">
         <v>149</v>
       </c>
       <c r="H46" t="s">
         <v>149</v>
       </c>
-      <c r="J46" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="K46" s="11" t="s">
+      <c r="J46" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="K46" s="10" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="47" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
         <v>103</v>
       </c>
@@ -2672,22 +2682,22 @@
         <v>18</v>
       </c>
       <c r="F47" t="s">
-        <v>183</v>
-      </c>
-      <c r="G47" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="G47" s="8" t="s">
         <v>154</v>
       </c>
-      <c r="H47" s="9" t="s">
-        <v>194</v>
-      </c>
-      <c r="J47" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="K47" s="11" t="s">
+      <c r="H47" s="8" t="s">
+        <v>190</v>
+      </c>
+      <c r="J47" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="K47" s="10" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="48" spans="2:11" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:11" ht="60" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
         <v>105</v>
       </c>
@@ -2697,17 +2707,17 @@
       <c r="D48" t="s">
         <v>13</v>
       </c>
-      <c r="F48" s="13" t="s">
+      <c r="F48" s="12" t="s">
         <v>145</v>
       </c>
-      <c r="G48" s="9" t="s">
-        <v>159</v>
-      </c>
-      <c r="H48" s="8" t="s">
-        <v>206</v>
-      </c>
-      <c r="I48" s="8" t="s">
-        <v>207</v>
+      <c r="G48" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="H48" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="I48" s="7" t="s">
+        <v>198</v>
       </c>
       <c r="J48" t="s">
         <v>151</v>
@@ -2716,7 +2726,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="49" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
         <v>107</v>
       </c>
@@ -2726,24 +2736,24 @@
       <c r="D49" t="s">
         <v>18</v>
       </c>
-      <c r="F49" s="16" t="s">
-        <v>184</v>
-      </c>
-      <c r="G49" s="9" t="s">
+      <c r="F49" s="15" t="s">
+        <v>181</v>
+      </c>
+      <c r="G49" s="8" t="s">
         <v>154</v>
       </c>
-      <c r="H49" s="9" t="s">
-        <v>196</v>
-      </c>
-      <c r="I49" s="10"/>
-      <c r="J49" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="K49" s="11" t="s">
+      <c r="H49" s="8" t="s">
+        <v>191</v>
+      </c>
+      <c r="I49" s="9"/>
+      <c r="J49" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="K49" s="10" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="50" spans="2:11" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:11" ht="60" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
         <v>109</v>
       </c>
@@ -2753,23 +2763,23 @@
       <c r="D50" t="s">
         <v>13</v>
       </c>
-      <c r="F50" s="15" t="s">
+      <c r="F50" s="14" t="s">
         <v>146</v>
       </c>
-      <c r="G50" s="9" t="s">
-        <v>159</v>
-      </c>
-      <c r="H50" s="8" t="s">
-        <v>197</v>
+      <c r="G50" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="H50" s="7" t="s">
+        <v>217</v>
       </c>
       <c r="J50" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="K50" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="51" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
         <v>111</v>
       </c>
@@ -2779,24 +2789,24 @@
       <c r="D51" t="s">
         <v>18</v>
       </c>
-      <c r="F51" s="16" t="s">
-        <v>185</v>
-      </c>
-      <c r="G51" s="9" t="s">
+      <c r="F51" s="15" t="s">
+        <v>182</v>
+      </c>
+      <c r="G51" s="8" t="s">
         <v>154</v>
       </c>
-      <c r="H51" s="9" t="s">
-        <v>199</v>
-      </c>
-      <c r="I51" s="12"/>
-      <c r="J51" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="K51" s="11" t="s">
+      <c r="H51" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="I51" s="11"/>
+      <c r="J51" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="K51" s="10" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="52" spans="2:11" ht="72" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:11" ht="75" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
         <v>113</v>
       </c>
@@ -2806,26 +2816,26 @@
       <c r="D52" t="s">
         <v>13</v>
       </c>
-      <c r="F52" s="14" t="s">
+      <c r="F52" s="13" t="s">
         <v>147</v>
       </c>
-      <c r="G52" s="9" t="s">
-        <v>159</v>
-      </c>
-      <c r="H52" s="8" t="s">
-        <v>201</v>
-      </c>
-      <c r="I52" s="8" t="s">
-        <v>200</v>
-      </c>
-      <c r="J52" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="K52" s="11" t="s">
+      <c r="G52" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="H52" s="7" t="s">
+        <v>218</v>
+      </c>
+      <c r="I52" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="J52" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="K52" s="10" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="53" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
         <v>115</v>
       </c>
@@ -2835,24 +2845,24 @@
       <c r="D53" t="s">
         <v>18</v>
       </c>
-      <c r="F53" s="16" t="s">
-        <v>186</v>
-      </c>
-      <c r="G53" s="9" t="s">
+      <c r="F53" s="15" t="s">
+        <v>183</v>
+      </c>
+      <c r="G53" s="8" t="s">
         <v>154</v>
       </c>
-      <c r="H53" s="9" t="s">
-        <v>202</v>
-      </c>
-      <c r="I53" s="12"/>
-      <c r="J53" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="K53" s="11" t="s">
+      <c r="H53" s="8" t="s">
+        <v>195</v>
+      </c>
+      <c r="I53" s="11"/>
+      <c r="J53" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="K53" s="10" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="54" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
         <v>117</v>
       </c>
@@ -2862,8 +2872,8 @@
       <c r="D54" t="s">
         <v>13</v>
       </c>
-      <c r="F54" s="6" t="s">
-        <v>216</v>
+      <c r="F54" s="15" t="s">
+        <v>210</v>
       </c>
       <c r="G54" s="2" t="s">
         <v>149</v>
@@ -2872,16 +2882,16 @@
         <v>149</v>
       </c>
       <c r="I54" t="s">
-        <v>215</v>
-      </c>
-      <c r="J54" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="K54" s="11" t="s">
+        <v>206</v>
+      </c>
+      <c r="J54" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="K54" s="10" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="55" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
         <v>119</v>
       </c>
@@ -2891,7 +2901,7 @@
       <c r="D55" t="s">
         <v>121</v>
       </c>
-      <c r="F55" s="16" t="s">
+      <c r="F55" s="15" t="s">
         <v>134</v>
       </c>
       <c r="G55" s="3" t="s">
@@ -2900,15 +2910,15 @@
       <c r="H55" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="I55" s="16"/>
-      <c r="J55" s="11" t="s">
-        <v>134</v>
-      </c>
-      <c r="K55" s="11" t="s">
+      <c r="I55" s="15"/>
+      <c r="J55" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="K55" s="10" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="56" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
         <v>122</v>
       </c>
@@ -2918,14 +2928,14 @@
       <c r="D56" t="s">
         <v>18</v>
       </c>
-      <c r="F56" s="16" t="s">
-        <v>212</v>
+      <c r="F56" s="15" t="s">
+        <v>203</v>
       </c>
       <c r="G56" s="2" t="s">
         <v>154</v>
       </c>
       <c r="H56" s="2" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="J56" s="2" t="s">
         <v>134</v>
@@ -2934,7 +2944,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="57" spans="2:11" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:11" ht="60" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
         <v>124</v>
       </c>
@@ -2945,25 +2955,25 @@
         <v>13</v>
       </c>
       <c r="F57" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="G57" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="H57" s="13" t="s">
-        <v>203</v>
-      </c>
-      <c r="I57" s="8" t="s">
-        <v>161</v>
-      </c>
-      <c r="J57" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="K57" s="11" t="s">
+      <c r="H57" s="12" t="s">
+        <v>196</v>
+      </c>
+      <c r="I57" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="J57" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="K57" s="10" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="58" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
         <v>126</v>
       </c>
@@ -2973,8 +2983,8 @@
       <c r="D58" t="s">
         <v>18</v>
       </c>
-      <c r="F58" s="16" t="s">
-        <v>214</v>
+      <c r="F58" s="15" t="s">
+        <v>205</v>
       </c>
       <c r="G58" s="2" t="s">
         <v>149</v>
@@ -2989,7 +2999,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="59" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
         <v>128</v>
       </c>
@@ -3009,7 +3019,7 @@
         <v>134</v>
       </c>
       <c r="I59" s="2" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
       <c r="J59" s="2" t="s">
         <v>134</v>
@@ -3018,7 +3028,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="60" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
         <v>130</v>
       </c>
@@ -3038,7 +3048,7 @@
         <v>134</v>
       </c>
       <c r="I60" s="2" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
       <c r="J60" s="2" t="s">
         <v>134</v>
@@ -3047,7 +3057,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="61" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
         <v>132</v>
       </c>
@@ -3058,12 +3068,12 @@
         <v>18</v>
       </c>
       <c r="F61" s="3" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="G61" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="H61" s="16" t="s">
+      <c r="H61" s="15" t="s">
         <v>149</v>
       </c>
       <c r="I61" s="5"/>

</xml_diff>

<commit_message>
EPICP-1 changed menopausal status recoding in DPE_EPICP_TRACY
</commit_message>
<xml_diff>
--- a/analyst/Tracy/rmonize/data_proc_elem/DPE_EPICP_TRACY.xlsx
+++ b/analyst/Tracy/rmonize/data_proc_elem/DPE_EPICP_TRACY.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Projekte\NFDI4Health\TA5\Pilotprojekte\Harmonisierung\HarmonizR\use-cases-harmonisation\analyst\Tracy\rmonize\data_proc_elem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F1D4D12-BA5C-465C-BCEA-02A87349F120}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{3FA55FF0-6FF8-4ED0-84C5-3DBF10CA98C3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -494,13 +494,6 @@
     <t>partial</t>
   </si>
   <si>
-    <t>pre-and perimenopausal can't be distinguished
-0=surgically induced menopause
-1= pre- or perimenopausal
-2=postmenopausal
-9= undefinable</t>
-  </si>
-  <si>
     <t>case_when</t>
   </si>
   <si>
@@ -917,9 +910,6 @@
     <t>inccanc_fup5</t>
   </si>
   <si>
-    <t>recode(0=3; 1=0; 1=2; 2=1; 9=NA)</t>
-  </si>
-  <si>
     <t>case_when(
 prevmi == 0 | prevstroke == 0  ~ 0L,
 prevmi == 1 | prevstroke == 1 ~ 1L, 
@@ -972,6 +962,12 @@
   </si>
   <si>
     <t>educc7;abschlus</t>
+  </si>
+  <si>
+    <t>recode(0=3; 1=0; 2=1; 9=NA)</t>
+  </si>
+  <si>
+    <t>no distinction between pre- and perimenopausal possible, hence this was mapped to premenopausal category in harmonized variable</t>
   </si>
 </sst>
 </file>
@@ -1425,8 +1421,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B43" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H58" sqref="H58"/>
+    <sheetView tabSelected="1" topLeftCell="B4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1514,7 +1510,7 @@
         <v>13</v>
       </c>
       <c r="F3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G3" t="s">
         <v>149</v>
@@ -1540,7 +1536,7 @@
         <v>18</v>
       </c>
       <c r="F4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="G4" t="s">
         <v>149</v>
@@ -1566,13 +1562,13 @@
         <v>13</v>
       </c>
       <c r="F5" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="G5" t="s">
         <v>150</v>
       </c>
       <c r="H5" s="17" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="J5" t="s">
         <v>151</v>
@@ -1592,7 +1588,7 @@
         <v>18</v>
       </c>
       <c r="F6" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="G6" t="s">
         <v>149</v>
@@ -1618,7 +1614,7 @@
         <v>13</v>
       </c>
       <c r="F7" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G7" t="s">
         <v>149</v>
@@ -1644,13 +1640,13 @@
         <v>13</v>
       </c>
       <c r="F8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G8" t="s">
         <v>150</v>
       </c>
       <c r="H8" s="15" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="J8" t="s">
         <v>151</v>
@@ -1748,13 +1744,13 @@
         <v>18</v>
       </c>
       <c r="F12" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>154</v>
       </c>
       <c r="H12" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="J12" s="2" t="s">
         <v>151</v>
@@ -1774,13 +1770,13 @@
         <v>18</v>
       </c>
       <c r="F13" s="16" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>154</v>
       </c>
       <c r="H13" s="15" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="J13" s="2" t="s">
         <v>151</v>
@@ -1800,7 +1796,7 @@
         <v>13</v>
       </c>
       <c r="F14" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>149</v>
@@ -1815,7 +1811,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>39</v>
       </c>
@@ -1826,22 +1822,22 @@
         <v>13</v>
       </c>
       <c r="F15" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>150</v>
       </c>
       <c r="H15" s="6" t="s">
-        <v>211</v>
+        <v>219</v>
       </c>
       <c r="I15" s="7" t="s">
-        <v>157</v>
+        <v>220</v>
       </c>
       <c r="J15" s="2" t="s">
         <v>156</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -1855,7 +1851,7 @@
         <v>13</v>
       </c>
       <c r="F16" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G16" s="2" t="s">
         <v>149</v>
@@ -1881,7 +1877,7 @@
         <v>13</v>
       </c>
       <c r="F17" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G17" s="2" t="s">
         <v>149</v>
@@ -1907,16 +1903,16 @@
         <v>13</v>
       </c>
       <c r="F18" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G18" t="s">
         <v>154</v>
       </c>
       <c r="H18" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="I18" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="J18" t="s">
         <v>151</v>
@@ -1936,7 +1932,7 @@
         <v>18</v>
       </c>
       <c r="F19" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="G19" t="s">
         <v>149</v>
@@ -2014,13 +2010,13 @@
         <v>13</v>
       </c>
       <c r="F22" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H22" s="12" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="J22" t="s">
         <v>151</v>
@@ -2326,7 +2322,7 @@
         <v>13</v>
       </c>
       <c r="F34" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G34" s="2" t="s">
         <v>149</v>
@@ -2352,7 +2348,7 @@
         <v>13</v>
       </c>
       <c r="F35" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="G35" s="2" t="s">
         <v>149</v>
@@ -2381,13 +2377,13 @@
         <v>140</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H36" s="12" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="I36" s="5" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="J36" s="2" t="s">
         <v>151</v>
@@ -2407,13 +2403,13 @@
         <v>18</v>
       </c>
       <c r="F37" s="13" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G37" s="2" t="s">
         <v>154</v>
       </c>
       <c r="H37" s="12" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="J37" s="2" t="s">
         <v>151</v>
@@ -2442,7 +2438,7 @@
         <v>135</v>
       </c>
       <c r="I38" s="9" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="J38" s="2" t="s">
         <v>134</v>
@@ -2492,13 +2488,13 @@
         <v>141</v>
       </c>
       <c r="G40" s="8" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H40" s="13" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="I40" s="9" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="J40" s="10" t="s">
         <v>151</v>
@@ -2518,13 +2514,13 @@
         <v>18</v>
       </c>
       <c r="F41" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G41" s="8" t="s">
         <v>154</v>
       </c>
       <c r="H41" s="8" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="I41" s="11"/>
       <c r="J41" s="10" t="s">
@@ -2548,13 +2544,13 @@
         <v>142</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H42" s="12" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="I42" s="5" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="J42" s="2" t="s">
         <v>151</v>
@@ -2574,13 +2570,13 @@
         <v>18</v>
       </c>
       <c r="F43" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G43" s="8" t="s">
         <v>154</v>
       </c>
       <c r="H43" s="8" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="I43" s="11"/>
       <c r="J43" s="10" t="s">
@@ -2610,7 +2606,7 @@
         <v>149</v>
       </c>
       <c r="I44" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="J44" s="10" t="s">
         <v>151</v>
@@ -2630,13 +2626,13 @@
         <v>18</v>
       </c>
       <c r="F45" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G45" s="8" t="s">
         <v>154</v>
       </c>
       <c r="H45" s="8" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="J45" s="10" t="s">
         <v>151</v>
@@ -2682,13 +2678,13 @@
         <v>18</v>
       </c>
       <c r="F47" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G47" s="8" t="s">
         <v>154</v>
       </c>
       <c r="H47" s="8" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="J47" s="10" t="s">
         <v>151</v>
@@ -2711,13 +2707,13 @@
         <v>145</v>
       </c>
       <c r="G48" s="8" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H48" s="7" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="I48" s="7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="J48" t="s">
         <v>151</v>
@@ -2737,13 +2733,13 @@
         <v>18</v>
       </c>
       <c r="F49" s="15" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G49" s="8" t="s">
         <v>154</v>
       </c>
       <c r="H49" s="8" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="I49" s="9"/>
       <c r="J49" s="10" t="s">
@@ -2767,13 +2763,13 @@
         <v>146</v>
       </c>
       <c r="G50" s="8" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H50" s="7" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="J50" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="K50" t="s">
         <v>153</v>
@@ -2790,13 +2786,13 @@
         <v>18</v>
       </c>
       <c r="F51" s="15" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G51" s="8" t="s">
         <v>154</v>
       </c>
       <c r="H51" s="8" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I51" s="11"/>
       <c r="J51" s="10" t="s">
@@ -2820,13 +2816,13 @@
         <v>147</v>
       </c>
       <c r="G52" s="8" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H52" s="7" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="I52" s="7" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="J52" s="10" t="s">
         <v>151</v>
@@ -2846,13 +2842,13 @@
         <v>18</v>
       </c>
       <c r="F53" s="15" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G53" s="8" t="s">
         <v>154</v>
       </c>
       <c r="H53" s="8" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="I53" s="11"/>
       <c r="J53" s="10" t="s">
@@ -2873,7 +2869,7 @@
         <v>13</v>
       </c>
       <c r="F54" s="15" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G54" s="2" t="s">
         <v>149</v>
@@ -2882,7 +2878,7 @@
         <v>149</v>
       </c>
       <c r="I54" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J54" s="10" t="s">
         <v>151</v>
@@ -2929,13 +2925,13 @@
         <v>18</v>
       </c>
       <c r="F56" s="15" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G56" s="2" t="s">
         <v>154</v>
       </c>
       <c r="H56" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="J56" s="2" t="s">
         <v>134</v>
@@ -2955,16 +2951,16 @@
         <v>13</v>
       </c>
       <c r="F57" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G57" s="4" t="s">
         <v>150</v>
       </c>
       <c r="H57" s="12" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="I57" s="7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="J57" s="10" t="s">
         <v>151</v>
@@ -2984,7 +2980,7 @@
         <v>18</v>
       </c>
       <c r="F58" s="15" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="G58" s="2" t="s">
         <v>149</v>
@@ -3019,7 +3015,7 @@
         <v>134</v>
       </c>
       <c r="I59" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="J59" s="2" t="s">
         <v>134</v>
@@ -3048,7 +3044,7 @@
         <v>134</v>
       </c>
       <c r="I60" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="J60" s="2" t="s">
         <v>134</v>
@@ -3068,7 +3064,7 @@
         <v>18</v>
       </c>
       <c r="F61" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G61" s="4" t="s">
         <v>149</v>

</xml_diff>

<commit_message>
removed spaces for variables in input_variables column
</commit_message>
<xml_diff>
--- a/analyst/Tracy/rmonize/data_proc_elem/DPE_EPICP_TRACY.xlsx
+++ b/analyst/Tracy/rmonize/data_proc_elem/DPE_EPICP_TRACY.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Projekte\NFDI4Health\TA5\Pilotprojekte\Harmonisierung\HarmonizR\use-cases-harmonisation\analyst\Tracy\rmonize\data_proc_elem\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schwarz-f\Desktop\use-cases-harmonisation\analyst\Tracy\rmonize\data_proc_elem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99FD4B0C-C3CA-4010-8200-16F227AC68FF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A169C0C0-791F-4CA0-B531-BAD4E8046EC9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="12" windowWidth="16092" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -818,6 +818,22 @@
 TRUE ~ 0)</t>
   </si>
   <si>
+    <t>age0 + (ysmkces0- format(as.Date(d_recrui, format="%d/%m/%Y"),"%Y")</t>
+  </si>
+  <si>
+    <t>kinder;ff10</t>
+  </si>
+  <si>
+    <t>kinder-ff10</t>
+  </si>
+  <si>
+    <t>age0 + ((dd_incmi - d_recrui)/365.25)
+age0 + ((dd_incstroke - d_recrui)/365.25)</t>
+  </si>
+  <si>
+    <r>
+      <t>age0 + ((</t>
+    </r>
     <r>
       <rPr>
         <sz val="11"/>
@@ -825,7 +841,106 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>age0; d_recrui;</t>
+      <t xml:space="preserve">dd_incmi </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>- d_recrui)/365.25)</t>
+    </r>
+  </si>
+  <si>
+    <t>age0;d_recrui;dd_incstroke</t>
+  </si>
+  <si>
+    <t>age0;d_recrui;dd_incmi</t>
+  </si>
+  <si>
+    <t>age0;d_recrui;dd_incmi;dd_incstroke</t>
+  </si>
+  <si>
+    <r>
+      <t>age0 + ((</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>dd_incstroke</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - d_recrui)/365.25)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>age0 + ((</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>dd_inchyp - d_recrui</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)/365.25)</t>
+    </r>
+  </si>
+  <si>
+    <t>age0 + ((ddinccanc - d_recrui)/365.25)</t>
+  </si>
+  <si>
+    <t>age0 + ((dd_incdiab - d_recrui)/365.25)</t>
+  </si>
+  <si>
+    <t>age0 + ((dd_inchf - d_recrui/365.25)</t>
+  </si>
+  <si>
+    <t>age0;d_recrui;dd_inccanc</t>
+  </si>
+  <si>
+    <t>age0;d_recrui;dd_incdiab</t>
+  </si>
+  <si>
+    <t>age0;d_recrui;dd_inchf</t>
+  </si>
+  <si>
+    <t>age0;d_recrui;dd_inchyp</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>age0;d_recrui;</t>
     </r>
     <r>
       <rPr>
@@ -847,121 +962,6 @@
       </rPr>
       <t>ysmkces0</t>
     </r>
-  </si>
-  <si>
-    <t>age0 + (ysmkces0- format(as.Date(d_recrui, format="%d/%m/%Y"),"%Y")</t>
-  </si>
-  <si>
-    <t>kinder;ff10</t>
-  </si>
-  <si>
-    <t>kinder-ff10</t>
-  </si>
-  <si>
-    <t>age0 + ((dd_incmi - d_recrui)/365.25)
-age0 + ((dd_incstroke - d_recrui)/365.25)</t>
-  </si>
-  <si>
-    <r>
-      <t>age0 + ((</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">dd_incmi </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>- d_recrui)/365.25)</t>
-    </r>
-  </si>
-  <si>
-    <t>age0;d_recrui;dd_incstroke</t>
-  </si>
-  <si>
-    <t>age0;d_recrui;dd_incmi</t>
-  </si>
-  <si>
-    <t>age0;d_recrui;dd_incmi;dd_incstroke</t>
-  </si>
-  <si>
-    <r>
-      <t>age0 + ((</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>dd_incstroke</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> - d_recrui)/365.25)</t>
-    </r>
-  </si>
-  <si>
-    <t>age0;d_recrui; dd_inchyp</t>
-  </si>
-  <si>
-    <r>
-      <t>age0 + ((</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>dd_inchyp - d_recrui</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>)/365.25)</t>
-    </r>
-  </si>
-  <si>
-    <t>age0;d_recrui; dd_inccanc</t>
-  </si>
-  <si>
-    <t>age0 + ((ddinccanc - d_recrui)/365.25)</t>
-  </si>
-  <si>
-    <t>age0 + ((dd_incdiab - d_recrui)/365.25)</t>
-  </si>
-  <si>
-    <t>age0;d_recrui; dd_incdiab</t>
-  </si>
-  <si>
-    <t>age0;d_recrui; dd_inchf</t>
-  </si>
-  <si>
-    <t>age0 + ((dd_inchf - d_recrui/365.25)</t>
   </si>
 </sst>
 </file>
@@ -1418,24 +1418,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H51" sqref="H51"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="46.5546875" customWidth="1"/>
-    <col min="5" max="5" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="73.88671875" customWidth="1"/>
-    <col min="9" max="9" width="54.5546875" customWidth="1"/>
-    <col min="10" max="10" width="18.109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="23.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="46.5703125" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="73.85546875" customWidth="1"/>
+    <col min="9" max="9" width="54.5703125" customWidth="1"/>
+    <col min="10" max="10" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="23.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1470,7 +1470,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>11</v>
       </c>
@@ -1496,7 +1496,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>14</v>
       </c>
@@ -1522,7 +1522,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>16</v>
       </c>
@@ -1548,7 +1548,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>19</v>
       </c>
@@ -1574,7 +1574,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>21</v>
       </c>
@@ -1600,7 +1600,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>23</v>
       </c>
@@ -1626,7 +1626,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>25</v>
       </c>
@@ -1652,7 +1652,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>27</v>
       </c>
@@ -1678,7 +1678,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>29</v>
       </c>
@@ -1704,7 +1704,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>31</v>
       </c>
@@ -1730,7 +1730,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B12" s="17" t="s">
         <v>33</v>
       </c>
@@ -1757,7 +1757,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>35</v>
       </c>
@@ -1768,13 +1768,13 @@
         <v>18</v>
       </c>
       <c r="F13" s="15" t="s">
-        <v>201</v>
+        <v>218</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>151</v>
       </c>
       <c r="H13" s="14" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="J13" s="2" t="s">
         <v>148</v>
@@ -1783,7 +1783,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>37</v>
       </c>
@@ -1809,7 +1809,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>39</v>
       </c>
@@ -1838,7 +1838,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>41</v>
       </c>
@@ -1864,7 +1864,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>43</v>
       </c>
@@ -1890,7 +1890,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>45</v>
       </c>
@@ -1901,13 +1901,13 @@
         <v>13</v>
       </c>
       <c r="F18" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G18" t="s">
         <v>151</v>
       </c>
       <c r="H18" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="I18" t="s">
         <v>178</v>
@@ -1919,7 +1919,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>47</v>
       </c>
@@ -1945,7 +1945,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="20" spans="2:11" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:11" ht="45" x14ac:dyDescent="0.25">
       <c r="B20" s="17" t="s">
         <v>49</v>
       </c>
@@ -1972,7 +1972,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="21" spans="2:11" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:11" ht="45" x14ac:dyDescent="0.25">
       <c r="B21" s="17" t="s">
         <v>51</v>
       </c>
@@ -1999,7 +1999,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="22" spans="2:11" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:11" ht="45" x14ac:dyDescent="0.25">
       <c r="B22" s="17" t="s">
         <v>53</v>
       </c>
@@ -2026,7 +2026,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B23" s="17" t="s">
         <v>55</v>
       </c>
@@ -2053,7 +2053,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B24" s="17" t="s">
         <v>57</v>
       </c>
@@ -2080,7 +2080,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>59</v>
       </c>
@@ -2106,7 +2106,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>61</v>
       </c>
@@ -2132,7 +2132,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>63</v>
       </c>
@@ -2158,7 +2158,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="28" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>65</v>
       </c>
@@ -2184,7 +2184,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="29" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>67</v>
       </c>
@@ -2210,7 +2210,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="30" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>69</v>
       </c>
@@ -2236,7 +2236,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="31" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>71</v>
       </c>
@@ -2262,7 +2262,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="32" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>73</v>
       </c>
@@ -2288,7 +2288,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="33" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>75</v>
       </c>
@@ -2314,7 +2314,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="34" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>77</v>
       </c>
@@ -2340,7 +2340,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="35" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>79</v>
       </c>
@@ -2366,7 +2366,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="36" spans="2:11" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:11" ht="90" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>81</v>
       </c>
@@ -2395,7 +2395,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="37" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>83</v>
       </c>
@@ -2406,13 +2406,13 @@
         <v>18</v>
       </c>
       <c r="F37" s="12" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="G37" s="2" t="s">
         <v>151</v>
       </c>
       <c r="H37" s="11" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="J37" s="2" t="s">
         <v>148</v>
@@ -2421,7 +2421,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="38" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>85</v>
       </c>
@@ -2450,7 +2450,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="39" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>87</v>
       </c>
@@ -2477,7 +2477,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="40" spans="2:11" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:11" ht="60" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>89</v>
       </c>
@@ -2506,7 +2506,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="41" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>91</v>
       </c>
@@ -2517,13 +2517,13 @@
         <v>18</v>
       </c>
       <c r="F41" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="G41" s="7" t="s">
         <v>151</v>
       </c>
       <c r="H41" s="7" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="I41" s="10"/>
       <c r="J41" s="9" t="s">
@@ -2533,7 +2533,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="42" spans="2:11" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:11" ht="60" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
         <v>93</v>
       </c>
@@ -2562,7 +2562,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="43" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
         <v>95</v>
       </c>
@@ -2573,13 +2573,13 @@
         <v>18</v>
       </c>
       <c r="F43" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="G43" s="7" t="s">
         <v>151</v>
       </c>
       <c r="H43" s="7" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="I43" s="10"/>
       <c r="J43" s="9" t="s">
@@ -2589,7 +2589,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="44" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
         <v>97</v>
       </c>
@@ -2618,7 +2618,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="45" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
         <v>99</v>
       </c>
@@ -2629,13 +2629,13 @@
         <v>18</v>
       </c>
       <c r="F45" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="G45" s="7" t="s">
         <v>151</v>
       </c>
       <c r="H45" s="7" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="J45" s="9" t="s">
         <v>148</v>
@@ -2644,7 +2644,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="46" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
         <v>101</v>
       </c>
@@ -2670,7 +2670,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="47" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
         <v>103</v>
       </c>
@@ -2681,13 +2681,13 @@
         <v>18</v>
       </c>
       <c r="F47" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="G47" s="7" t="s">
         <v>151</v>
       </c>
       <c r="H47" s="7" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="J47" s="9" t="s">
         <v>148</v>
@@ -2696,7 +2696,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="48" spans="2:11" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:11" ht="60" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
         <v>105</v>
       </c>
@@ -2725,7 +2725,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="49" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
         <v>107</v>
       </c>
@@ -2736,13 +2736,13 @@
         <v>18</v>
       </c>
       <c r="F49" s="14" t="s">
-        <v>211</v>
+        <v>217</v>
       </c>
       <c r="G49" s="7" t="s">
         <v>151</v>
       </c>
       <c r="H49" s="7" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="I49" s="8"/>
       <c r="J49" s="9" t="s">
@@ -2752,7 +2752,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="50" spans="2:11" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:11" ht="60" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
         <v>109</v>
       </c>
@@ -2778,7 +2778,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="51" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
         <v>111</v>
       </c>
@@ -2789,13 +2789,13 @@
         <v>18</v>
       </c>
       <c r="F51" s="14" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G51" s="7" t="s">
         <v>151</v>
       </c>
       <c r="H51" s="7" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="I51" s="10"/>
       <c r="J51" s="9" t="s">
@@ -2805,7 +2805,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="52" spans="2:11" ht="72" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:11" ht="75" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
         <v>113</v>
       </c>
@@ -2834,7 +2834,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="53" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
         <v>115</v>
       </c>
@@ -2845,13 +2845,13 @@
         <v>18</v>
       </c>
       <c r="F53" s="14" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G53" s="7" t="s">
         <v>151</v>
       </c>
       <c r="H53" s="7" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="I53" s="10"/>
       <c r="J53" s="9" t="s">
@@ -2861,7 +2861,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="54" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
         <v>117</v>
       </c>
@@ -2890,7 +2890,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="55" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
         <v>119</v>
       </c>
@@ -2917,7 +2917,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="56" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
         <v>122</v>
       </c>
@@ -2928,13 +2928,13 @@
         <v>18</v>
       </c>
       <c r="F56" s="14" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="G56" s="2" t="s">
         <v>151</v>
       </c>
       <c r="H56" s="2" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="J56" s="2" t="s">
         <v>134</v>
@@ -2943,7 +2943,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="57" spans="2:11" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:11" ht="60" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
         <v>124</v>
       </c>
@@ -2972,7 +2972,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="58" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
         <v>126</v>
       </c>
@@ -2998,7 +2998,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="59" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
         <v>128</v>
       </c>
@@ -3027,7 +3027,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="60" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
         <v>130</v>
       </c>
@@ -3056,7 +3056,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="61" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
         <v>132</v>
       </c>

</xml_diff>

<commit_message>
age cancer and hf adjustments
</commit_message>
<xml_diff>
--- a/analyst/Tracy/rmonize/data_proc_elem/DPE_EPICP_TRACY.xlsx
+++ b/analyst/Tracy/rmonize/data_proc_elem/DPE_EPICP_TRACY.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schwarz-f\Desktop\use-cases-harmonisation\analyst\Tracy\rmonize\data_proc_elem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E90B6465-EA5D-43DA-8E2D-64DBC30C146B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{548C5AED-B2B9-48E1-B138-4A60E0812505}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -948,12 +948,6 @@
     <t>age0 + (as.numeric(as.Date(paste0(ysmkces0, "-06-30")))-as.numeric(d_recrui))/365.25</t>
   </si>
   <si>
-    <t>age0 + (as.numeric(as.Date(paste0(dd_inchf, "-06-30")))-as.numeric(d_recrui))/365.25</t>
-  </si>
-  <si>
-    <t>age0 + (as.numeric(as.Date(paste0(dd_inccanc, "-06-30")))-as.numeric(d_recrui))/365.25</t>
-  </si>
-  <si>
     <t>case_when(
 casemi_fup5 %in% c(0) ~ 0L,
 casemi_fup5 %in% c(2,5) ~ 1L,
@@ -961,6 +955,54 @@
   </si>
   <si>
     <t>min(age0 + ((dd_incmi - d_recrui)/365.25),age0 + ((dd_incstroke - d_recrui)/365.25), na.rm = TRUE)</t>
+  </si>
+  <si>
+    <r>
+      <t>age0 + ((</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>dd_inchf - d_recrui</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)/365.25)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>age0 + ((</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>dd_inccanc - d_recrui</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)/365.25)</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1417,8 +1459,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H38" sqref="H38"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="H57" sqref="H57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2411,7 +2453,7 @@
         <v>151</v>
       </c>
       <c r="H37" s="11" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="J37" s="2" t="s">
         <v>148</v>
@@ -2493,7 +2535,7 @@
         <v>154</v>
       </c>
       <c r="H40" s="12" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="I40" s="8" t="s">
         <v>178</v>
@@ -2794,7 +2836,7 @@
         <v>151</v>
       </c>
       <c r="H51" s="7" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="I51" s="10"/>
       <c r="J51" s="9" t="s">
@@ -2916,7 +2958,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="56" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
         <v>122</v>
       </c>
@@ -2932,8 +2974,8 @@
       <c r="G56" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="H56" s="2" t="s">
-        <v>216</v>
+      <c r="H56" s="7" t="s">
+        <v>218</v>
       </c>
       <c r="J56" s="2" t="s">
         <v>134</v>

</xml_diff>

<commit_message>
Tracy na.rm for operation
</commit_message>
<xml_diff>
--- a/analyst/Tracy/rmonize/data_proc_elem/DPE_EPICP_TRACY.xlsx
+++ b/analyst/Tracy/rmonize/data_proc_elem/DPE_EPICP_TRACY.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schwarz-f\Desktop\use-cases-harmonisation\analyst\Tracy\rmonize\data_proc_elem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{548C5AED-B2B9-48E1-B138-4A60E0812505}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BBC06A2-7F59-41DE-A1B8-417D64D55491}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -942,9 +942,6 @@
     <t>zt3;zr3;pf3</t>
   </si>
   <si>
-    <t>(zt3*1) + (zr3*5) + (pf3*5)</t>
-  </si>
-  <si>
     <t>age0 + (as.numeric(as.Date(paste0(ysmkces0, "-06-30")))-as.numeric(d_recrui))/365.25</t>
   </si>
   <si>
@@ -1003,6 +1000,9 @@
       </rPr>
       <t>)/365.25)</t>
     </r>
+  </si>
+  <si>
+    <t>sum((zt3*1), (zr3*5),(pf3*5), na.rm = TRUE)</t>
   </si>
 </sst>
 </file>
@@ -1459,8 +1459,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H57" sqref="H57"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1789,7 +1789,7 @@
         <v>151</v>
       </c>
       <c r="H12" s="17" t="s">
-        <v>213</v>
+        <v>218</v>
       </c>
       <c r="J12" s="2" t="s">
         <v>148</v>
@@ -1815,7 +1815,7 @@
         <v>151</v>
       </c>
       <c r="H13" s="14" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="J13" s="2" t="s">
         <v>148</v>
@@ -2453,7 +2453,7 @@
         <v>151</v>
       </c>
       <c r="H37" s="11" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="J37" s="2" t="s">
         <v>148</v>
@@ -2535,7 +2535,7 @@
         <v>154</v>
       </c>
       <c r="H40" s="12" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="I40" s="8" t="s">
         <v>178</v>
@@ -2836,7 +2836,7 @@
         <v>151</v>
       </c>
       <c r="H51" s="7" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="I51" s="10"/>
       <c r="J51" s="9" t="s">
@@ -2975,7 +2975,7 @@
         <v>151</v>
       </c>
       <c r="H56" s="7" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="J56" s="2" t="s">
         <v>134</v>

</xml_diff>

<commit_message>
finalising EPICP besides incident Q
</commit_message>
<xml_diff>
--- a/analyst/Tracy/rmonize/data_proc_elem/DPE_EPICP_TRACY.xlsx
+++ b/analyst/Tracy/rmonize/data_proc_elem/DPE_EPICP_TRACY.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schwarz-f\Desktop\use-cases-harmonisation\analyst\Tracy\rmonize\data_proc_elem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BBC06A2-7F59-41DE-A1B8-417D64D55491}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4202268D-0A96-4F4E-A19F-A4F36DEF927E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="220">
   <si>
     <t>index</t>
   </si>
@@ -738,35 +738,6 @@
   </si>
   <si>
     <t>case_when(
-casemi_fup5 %in% c(0) | casestroke_fup5 %in% c(0) | casehf_fup5 %in% c(0) ~ 0L,
-casemi_fup5 %in% c(2,5) | casestroke_fup5 %in% c(2,6) | casehf_fup5 == 2 ~ 1L, TRUE ~ NA_integer_)</t>
-  </si>
-  <si>
-    <t>case_when(
-casestroke_fup5 %in% c(0) ~ 0L,
-casestroke_fup5 %in% c(2,6) ~ 1L,
-TRUE ~ NA_integer_)</t>
-  </si>
-  <si>
-    <t>case_when(
-casehyp_fup5 == 0 ~ 0L,
-casehyp_fup5 == 2 ~ 1L,
-TRUE ~ NA_integer_)</t>
-  </si>
-  <si>
-    <t>case_when(
-casehf_fup5 == 0 ~ 0L,
-casehf_fup5 == 2 ~ 1L,
-TRUE ~ NA_integer_)</t>
-  </si>
-  <si>
-    <t>case_when(
-casediab_fup5 == 0 ~ 0L,
-casediab_fup5 == 2 ~ 1L,
-TRUE ~ NA_integer_)</t>
-  </si>
-  <si>
-    <t>case_when(
 educc7 %in% c(7) ~ 7L,
 educc7 %in% c(5,6) ~ 6L,
 educc7 %in% c(3,4) ~ 4L,
@@ -798,15 +769,7 @@
 TRUE ~ 0)</t>
   </si>
   <si>
-    <t>case_when(
-casemi_fup5 == 1 | casestroke_fup5 == 1 ~ 1L,
-TRUE ~ 0)</t>
-  </si>
-  <si>
     <t>kinder;ff10</t>
-  </si>
-  <si>
-    <t>kinder-ff10</t>
   </si>
   <si>
     <r>
@@ -837,9 +800,6 @@
   </si>
   <si>
     <t>age0;d_recrui;dd_incmi</t>
-  </si>
-  <si>
-    <t>age0;d_recrui;dd_incmi;dd_incstroke</t>
   </si>
   <si>
     <r>
@@ -945,15 +905,6 @@
     <t>age0 + (as.numeric(as.Date(paste0(ysmkces0, "-06-30")))-as.numeric(d_recrui))/365.25</t>
   </si>
   <si>
-    <t>case_when(
-casemi_fup5 %in% c(0) ~ 0L,
-casemi_fup5 %in% c(2,5) ~ 1L,
-TRUE ~ NA_integer_)</t>
-  </si>
-  <si>
-    <t>min(age0 + ((dd_incmi - d_recrui)/365.25),age0 + ((dd_incstroke - d_recrui)/365.25), na.rm = TRUE)</t>
-  </si>
-  <si>
     <r>
       <t>age0 + ((</t>
     </r>
@@ -1002,7 +953,68 @@
     </r>
   </si>
   <si>
-    <t>sum((zt3*1), (zr3*5),(pf3*5), na.rm = TRUE)</t>
+    <t>ifelse(is.na(zt3),
+                      ifelse(is.na(zr3), 
+                             ifelse(is.na(pf3),0,pf3*5),
+                             ifelse(is.na(pf3),zr3*5,zr3*5+pf3*5)),
+                      ifelse(is.na(zr3),
+                             ifelse(is.na(pf3),zt3*1,zt3*1+pf3*5),
+                             ifelse(is.na(pf3),zt3*1+zr3*5, zt3*1+ zr3*5 + pf3*5)))</t>
+  </si>
+  <si>
+    <t>ifelse(is.na(kinder),
+                      ifelse(is.na(ff10),0,0),
+                      ifelse(is.na(ff10),kinder, kinder-ff10))</t>
+  </si>
+  <si>
+    <t>case_when(
+casemi_fup5 == 1 | casestroke_fup5 == 1 | casehf_fup5 == 1 ~ 1L,
+TRUE ~ 0L)</t>
+  </si>
+  <si>
+    <t>case_when(
+  casemi_fup5 %in% c(2,5) | casestroke_fup5 %in% c(2,6) | casehf_fup5 == 2 ~ 1L,
+  casemi_fup5 %in% c(0) | casestroke_fup5 %in% c(0) | casehf_fup5 %in% c(0) ~ 0L,
+  TRUE ~ NA_integer_)</t>
+  </si>
+  <si>
+    <t>casemi_fup5;casestroke_fup5;casehf_fup5</t>
+  </si>
+  <si>
+    <t>age0;d_recrui;dd_incmi;dd_incstroke;dd_inchf</t>
+  </si>
+  <si>
+    <t>min(age0 + ((dd_incmi - d_recrui)/365.25),age0 + ((dd_incstroke - d_recrui)/365.25),age0 + ((dd_inchf - d_recrui)/365.25) na.rm = TRUE)</t>
+  </si>
+  <si>
+    <t>case_when(
+casemi_fup5 %in% c(2,5) ~ 1L,
+casemi_fup5 %in% c(0) ~ 0L,
+TRUE ~ NA_integer_)</t>
+  </si>
+  <si>
+    <t>case_when(
+casestroke_fup5 %in% c(2,6) ~ 1L,
+casestroke_fup5 %in% c(0) ~ 0L,
+TRUE ~ NA_integer_)</t>
+  </si>
+  <si>
+    <t>case_when(
+casehyp_fup5 == 2 ~ 1L,
+casehyp_fup5 == 0 ~ 0L,
+TRUE ~ NA_integer_)</t>
+  </si>
+  <si>
+    <t>case_when(
+casehf_fup5 == 2 ~ 1L,
+casehf_fup5 == 0 ~ 0L,
+TRUE ~ NA_integer_)</t>
+  </si>
+  <si>
+    <t>case_when(
+casediab_fup5 == 2 ~ 1L,
+casediab_fup5 == 0 ~ 0L,
+TRUE ~ NA_integer_)</t>
   </si>
 </sst>
 </file>
@@ -1073,7 +1085,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1119,6 +1131,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1459,8 +1472,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K61"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" topLeftCell="A50" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H57" sqref="H57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1600,13 +1613,13 @@
         <v>13</v>
       </c>
       <c r="F5" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="G5" t="s">
         <v>154</v>
       </c>
       <c r="H5" s="16" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="J5" t="s">
         <v>148</v>
@@ -1626,7 +1639,7 @@
         <v>18</v>
       </c>
       <c r="F6" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="G6" t="s">
         <v>146</v>
@@ -1783,13 +1796,13 @@
       </c>
       <c r="E12" s="17"/>
       <c r="F12" s="17" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="G12" s="18" t="s">
         <v>151</v>
       </c>
-      <c r="H12" s="17" t="s">
-        <v>218</v>
+      <c r="H12" s="19" t="s">
+        <v>208</v>
       </c>
       <c r="J12" s="2" t="s">
         <v>148</v>
@@ -1809,13 +1822,13 @@
         <v>18</v>
       </c>
       <c r="F13" s="15" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>151</v>
       </c>
       <c r="H13" s="14" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="J13" s="2" t="s">
         <v>148</v>
@@ -1867,10 +1880,10 @@
         <v>147</v>
       </c>
       <c r="H15" s="14" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="I15" s="6" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="J15" s="2" t="s">
         <v>153</v>
@@ -1931,7 +1944,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:11" ht="45" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>45</v>
       </c>
@@ -1942,13 +1955,13 @@
         <v>13</v>
       </c>
       <c r="F18" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="G18" t="s">
         <v>151</v>
       </c>
-      <c r="H18" t="s">
-        <v>198</v>
+      <c r="H18" s="6" t="s">
+        <v>209</v>
       </c>
       <c r="I18" t="s">
         <v>175</v>
@@ -2004,7 +2017,7 @@
         <v>154</v>
       </c>
       <c r="H20" s="10" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="J20" t="s">
         <v>148</v>
@@ -2031,7 +2044,7 @@
         <v>154</v>
       </c>
       <c r="H21" s="10" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="J21" t="s">
         <v>148</v>
@@ -2052,13 +2065,13 @@
       </c>
       <c r="E22" s="17"/>
       <c r="F22" s="17" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="G22" s="18" t="s">
         <v>154</v>
       </c>
       <c r="H22" s="12" t="s">
-        <v>196</v>
+        <v>210</v>
       </c>
       <c r="J22" t="s">
         <v>148</v>
@@ -2418,13 +2431,13 @@
         <v>13</v>
       </c>
       <c r="F36" s="12" t="s">
-        <v>193</v>
+        <v>212</v>
       </c>
       <c r="G36" s="2" t="s">
         <v>154</v>
       </c>
       <c r="H36" s="11" t="s">
-        <v>184</v>
+        <v>211</v>
       </c>
       <c r="I36" s="5" t="s">
         <v>157</v>
@@ -2447,13 +2460,13 @@
         <v>18</v>
       </c>
       <c r="F37" s="12" t="s">
-        <v>202</v>
+        <v>213</v>
       </c>
       <c r="G37" s="2" t="s">
         <v>151</v>
       </c>
       <c r="H37" s="11" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="J37" s="2" t="s">
         <v>148</v>
@@ -2535,7 +2548,7 @@
         <v>154</v>
       </c>
       <c r="H40" s="12" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="I40" s="8" t="s">
         <v>178</v>
@@ -2558,13 +2571,13 @@
         <v>18</v>
       </c>
       <c r="F41" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="G41" s="7" t="s">
         <v>151</v>
       </c>
       <c r="H41" s="7" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="I41" s="10"/>
       <c r="J41" s="9" t="s">
@@ -2591,7 +2604,7 @@
         <v>154</v>
       </c>
       <c r="H42" s="11" t="s">
-        <v>185</v>
+        <v>216</v>
       </c>
       <c r="I42" s="5" t="s">
         <v>177</v>
@@ -2614,13 +2627,13 @@
         <v>18</v>
       </c>
       <c r="F43" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="G43" s="7" t="s">
         <v>151</v>
       </c>
       <c r="H43" s="7" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="I43" s="10"/>
       <c r="J43" s="9" t="s">
@@ -2670,13 +2683,13 @@
         <v>18</v>
       </c>
       <c r="F45" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="G45" s="7" t="s">
         <v>151</v>
       </c>
       <c r="H45" s="7" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="J45" s="9" t="s">
         <v>148</v>
@@ -2722,13 +2735,13 @@
         <v>18</v>
       </c>
       <c r="F47" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="G47" s="7" t="s">
         <v>151</v>
       </c>
       <c r="H47" s="7" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="J47" s="9" t="s">
         <v>148</v>
@@ -2754,7 +2767,7 @@
         <v>154</v>
       </c>
       <c r="H48" s="6" t="s">
-        <v>186</v>
+        <v>217</v>
       </c>
       <c r="I48" s="6" t="s">
         <v>176</v>
@@ -2777,13 +2790,13 @@
         <v>18</v>
       </c>
       <c r="F49" s="14" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="G49" s="7" t="s">
         <v>151</v>
       </c>
       <c r="H49" s="7" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="I49" s="8"/>
       <c r="J49" s="9" t="s">
@@ -2810,7 +2823,7 @@
         <v>154</v>
       </c>
       <c r="H50" s="6" t="s">
-        <v>187</v>
+        <v>218</v>
       </c>
       <c r="J50" t="s">
         <v>172</v>
@@ -2830,13 +2843,13 @@
         <v>18</v>
       </c>
       <c r="F51" s="14" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="G51" s="7" t="s">
         <v>151</v>
       </c>
       <c r="H51" s="7" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
       <c r="I51" s="10"/>
       <c r="J51" s="9" t="s">
@@ -2863,7 +2876,7 @@
         <v>154</v>
       </c>
       <c r="H52" s="6" t="s">
-        <v>188</v>
+        <v>219</v>
       </c>
       <c r="I52" s="6" t="s">
         <v>173</v>
@@ -2886,13 +2899,13 @@
         <v>18</v>
       </c>
       <c r="F53" s="14" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
       <c r="G53" s="7" t="s">
         <v>151</v>
       </c>
       <c r="H53" s="7" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="I53" s="10"/>
       <c r="J53" s="9" t="s">
@@ -2969,13 +2982,13 @@
         <v>18</v>
       </c>
       <c r="F56" s="14" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
       <c r="G56" s="2" t="s">
         <v>151</v>
       </c>
       <c r="H56" s="7" t="s">
-        <v>217</v>
+        <v>207</v>
       </c>
       <c r="J56" s="2" t="s">
         <v>134</v>

</xml_diff>

<commit_message>
missing comma in AGE_CVD
</commit_message>
<xml_diff>
--- a/analyst/Tracy/rmonize/data_proc_elem/DPE_EPICP_TRACY.xlsx
+++ b/analyst/Tracy/rmonize/data_proc_elem/DPE_EPICP_TRACY.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schwarz-f\Desktop\use-cases-harmonisation\analyst\Tracy\rmonize\data_proc_elem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4202268D-0A96-4F4E-A19F-A4F36DEF927E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BCD61E8-9646-49DC-B5A5-0F183460EDF5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -984,9 +984,6 @@
     <t>age0;d_recrui;dd_incmi;dd_incstroke;dd_inchf</t>
   </si>
   <si>
-    <t>min(age0 + ((dd_incmi - d_recrui)/365.25),age0 + ((dd_incstroke - d_recrui)/365.25),age0 + ((dd_inchf - d_recrui)/365.25) na.rm = TRUE)</t>
-  </si>
-  <si>
     <t>case_when(
 casemi_fup5 %in% c(2,5) ~ 1L,
 casemi_fup5 %in% c(0) ~ 0L,
@@ -1015,6 +1012,9 @@
 casediab_fup5 == 2 ~ 1L,
 casediab_fup5 == 0 ~ 0L,
 TRUE ~ NA_integer_)</t>
+  </si>
+  <si>
+    <t>min(age0 + ((dd_incmi - d_recrui)/365.25),age0 + ((dd_incstroke - d_recrui)/365.25),age0 + ((dd_inchf - d_recrui)/365.25), na.rm = TRUE)</t>
   </si>
 </sst>
 </file>
@@ -1472,8 +1472,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H57" sqref="H57"/>
+    <sheetView tabSelected="1" topLeftCell="A35" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H37" sqref="H37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2466,7 +2466,7 @@
         <v>151</v>
       </c>
       <c r="H37" s="11" t="s">
-        <v>214</v>
+        <v>219</v>
       </c>
       <c r="J37" s="2" t="s">
         <v>148</v>
@@ -2548,7 +2548,7 @@
         <v>154</v>
       </c>
       <c r="H40" s="12" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="I40" s="8" t="s">
         <v>178</v>
@@ -2604,7 +2604,7 @@
         <v>154</v>
       </c>
       <c r="H42" s="11" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="I42" s="5" t="s">
         <v>177</v>
@@ -2767,7 +2767,7 @@
         <v>154</v>
       </c>
       <c r="H48" s="6" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="I48" s="6" t="s">
         <v>176</v>
@@ -2823,7 +2823,7 @@
         <v>154</v>
       </c>
       <c r="H50" s="6" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="J50" t="s">
         <v>172</v>
@@ -2876,7 +2876,7 @@
         <v>154</v>
       </c>
       <c r="H52" s="6" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="I52" s="6" t="s">
         <v>173</v>

</xml_diff>

<commit_message>
DPE_EPICP_TRACY pushed by Franzi for checking
</commit_message>
<xml_diff>
--- a/analyst/Tracy/rmonize/data_proc_elem/DPE_EPICP_TRACY.xlsx
+++ b/analyst/Tracy/rmonize/data_proc_elem/DPE_EPICP_TRACY.xlsx
@@ -5,22 +5,22 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schwarz-f\Desktop\use-cases-harmonisation\analyst\Tracy\rmonize\data_proc_elem\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Projekte\NFDI4Health\TA5\Pilotprojekte\Harmonisierung\HarmonizR\use-cases-harmonisation\analyst\Tracy\rmonize\data_proc_elem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD44B379-67E6-4121-B1C8-A03DF5156ADF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F18E7281-3198-44A7-A1EC-B61C702247F9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="222">
   <si>
     <t>index</t>
   </si>
@@ -614,9 +614,6 @@
     <t>recode(1=1; 2= 0; 6= 1)</t>
   </si>
   <si>
-    <t>number of children minus stillbirths</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">0=not diseased; 1= prevalent; 2=incident; </t>
     </r>
@@ -767,9 +764,6 @@
     <t>case_when(
 casehyp_fup5 == 1 ~ 1L,
 TRUE ~ 0)</t>
-  </si>
-  <si>
-    <t>kinder;ff10</t>
   </si>
   <si>
     <r>
@@ -962,11 +956,6 @@
                              ifelse(is.na(pf3),zt3*1+zr3*5, zt3*1+ zr3*5 + pf3*5)))</t>
   </si>
   <si>
-    <t>ifelse(is.na(kinder),
-                      ifelse(is.na(ff10),0,0),
-                      ifelse(is.na(ff10),kinder, kinder-ff10))</t>
-  </si>
-  <si>
     <t>case_when(
 casemi_fup5 == 1 | casestroke_fup5 == 1 | casehf_fup5 == 1 ~ 1L,
 TRUE ~ 0L)</t>
@@ -1027,6 +1016,15 @@
     <t>as.numeric(pmin(age0 + ((dd_inchf - d_recrui)/365.25),
                      age0 + ((dd_incstroke - d_recrui)/365.25),
                      age0 + ((dd_incmi - d_recrui)/365.25), na.rm = TRUE))</t>
+  </si>
+  <si>
+    <t>kinder</t>
+  </si>
+  <si>
+    <t>number of children as proxy for number of pregnancies</t>
+  </si>
+  <si>
+    <t>if inccanc_fup5=1, then take dd_inccanc; if inccanc_fup5 = 0, then take dcens_canc</t>
   </si>
 </sst>
 </file>
@@ -1077,12 +1075,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -1097,7 +1101,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1142,6 +1146,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1483,8 +1494,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H37" sqref="H37"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="I67" sqref="I67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1494,8 +1505,8 @@
     <col min="5" max="5" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="30.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="73.85546875" customWidth="1"/>
-    <col min="9" max="9" width="54.5703125" customWidth="1"/>
+    <col min="8" max="8" width="60.28515625" customWidth="1"/>
+    <col min="9" max="9" width="87.28515625" customWidth="1"/>
     <col min="10" max="10" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="23.85546875" bestFit="1" customWidth="1"/>
   </cols>
@@ -1624,13 +1635,13 @@
         <v>13</v>
       </c>
       <c r="F5" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G5" t="s">
         <v>154</v>
       </c>
       <c r="H5" s="16" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="J5" t="s">
         <v>148</v>
@@ -1650,7 +1661,7 @@
         <v>18</v>
       </c>
       <c r="F6" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="G6" t="s">
         <v>146</v>
@@ -1807,13 +1818,13 @@
       </c>
       <c r="E12" s="17"/>
       <c r="F12" s="17" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="G12" s="18" t="s">
         <v>151</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="J12" s="2" t="s">
         <v>148</v>
@@ -1833,13 +1844,13 @@
         <v>18</v>
       </c>
       <c r="F13" s="15" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>151</v>
       </c>
       <c r="H13" s="14" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="J13" s="2" t="s">
         <v>148</v>
@@ -1891,10 +1902,10 @@
         <v>147</v>
       </c>
       <c r="H15" s="14" t="s">
+        <v>185</v>
+      </c>
+      <c r="I15" s="6" t="s">
         <v>186</v>
-      </c>
-      <c r="I15" s="6" t="s">
-        <v>187</v>
       </c>
       <c r="J15" s="2" t="s">
         <v>153</v>
@@ -1929,7 +1940,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>43</v>
       </c>
@@ -1955,36 +1966,38 @@
         <v>149</v>
       </c>
     </row>
-    <row r="18" spans="2:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="19"/>
+      <c r="B18" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="D18" t="s">
-        <v>13</v>
-      </c>
-      <c r="F18" t="s">
-        <v>191</v>
-      </c>
-      <c r="G18" t="s">
-        <v>151</v>
-      </c>
-      <c r="H18" s="6" t="s">
-        <v>209</v>
-      </c>
-      <c r="I18" t="s">
-        <v>175</v>
-      </c>
-      <c r="J18" t="s">
-        <v>148</v>
-      </c>
-      <c r="K18" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="D18" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="E18" s="19"/>
+      <c r="F18" s="19" t="s">
+        <v>219</v>
+      </c>
+      <c r="G18" s="19" t="s">
+        <v>146</v>
+      </c>
+      <c r="H18" s="20" t="s">
+        <v>146</v>
+      </c>
+      <c r="I18" s="19" t="s">
+        <v>220</v>
+      </c>
+      <c r="J18" s="19" t="s">
+        <v>153</v>
+      </c>
+      <c r="K18" s="19" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>47</v>
       </c>
@@ -2010,7 +2023,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="20" spans="2:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="B20" s="17" t="s">
         <v>49</v>
       </c>
@@ -2028,7 +2041,7 @@
         <v>154</v>
       </c>
       <c r="H20" s="10" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="J20" t="s">
         <v>148</v>
@@ -2037,7 +2050,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="21" spans="2:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="B21" s="17" t="s">
         <v>51</v>
       </c>
@@ -2055,7 +2068,7 @@
         <v>154</v>
       </c>
       <c r="H21" s="10" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="J21" t="s">
         <v>148</v>
@@ -2064,7 +2077,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="22" spans="2:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="B22" s="17" t="s">
         <v>53</v>
       </c>
@@ -2076,13 +2089,13 @@
       </c>
       <c r="E22" s="17"/>
       <c r="F22" s="17" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G22" s="18" t="s">
         <v>154</v>
       </c>
       <c r="H22" s="12" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="J22" t="s">
         <v>148</v>
@@ -2091,7 +2104,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B23" s="17" t="s">
         <v>55</v>
       </c>
@@ -2118,7 +2131,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B24" s="17" t="s">
         <v>57</v>
       </c>
@@ -2145,7 +2158,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>59</v>
       </c>
@@ -2171,7 +2184,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>61</v>
       </c>
@@ -2197,7 +2210,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>63</v>
       </c>
@@ -2223,7 +2236,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>65</v>
       </c>
@@ -2249,7 +2262,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>67</v>
       </c>
@@ -2275,7 +2288,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>69</v>
       </c>
@@ -2301,7 +2314,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="31" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>71</v>
       </c>
@@ -2327,7 +2340,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="32" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>73</v>
       </c>
@@ -2442,13 +2455,13 @@
         <v>13</v>
       </c>
       <c r="F36" s="12" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="G36" s="2" t="s">
         <v>154</v>
       </c>
       <c r="H36" s="11" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="I36" s="5" t="s">
         <v>157</v>
@@ -2471,13 +2484,13 @@
         <v>18</v>
       </c>
       <c r="F37" s="12" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="G37" s="2" t="s">
         <v>151</v>
       </c>
       <c r="H37" s="11" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="J37" s="2" t="s">
         <v>148</v>
@@ -2506,7 +2519,7 @@
         <v>135</v>
       </c>
       <c r="I38" s="8" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="J38" s="2" t="s">
         <v>134</v>
@@ -2559,10 +2572,10 @@
         <v>154</v>
       </c>
       <c r="H40" s="12" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="I40" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="J40" s="9" t="s">
         <v>148</v>
@@ -2582,13 +2595,13 @@
         <v>18</v>
       </c>
       <c r="F41" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="G41" s="7" t="s">
         <v>151</v>
       </c>
       <c r="H41" s="7" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="I41" s="10"/>
       <c r="J41" s="9" t="s">
@@ -2615,10 +2628,10 @@
         <v>154</v>
       </c>
       <c r="H42" s="11" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="I42" s="5" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="J42" s="2" t="s">
         <v>148</v>
@@ -2638,13 +2651,13 @@
         <v>18</v>
       </c>
       <c r="F43" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="G43" s="7" t="s">
         <v>151</v>
       </c>
       <c r="H43" s="7" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="I43" s="10"/>
       <c r="J43" s="9" t="s">
@@ -2671,7 +2684,7 @@
         <v>154</v>
       </c>
       <c r="H44" s="6" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="I44" t="s">
         <v>158</v>
@@ -2694,13 +2707,13 @@
         <v>18</v>
       </c>
       <c r="F45" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="G45" s="7" t="s">
         <v>151</v>
       </c>
       <c r="H45" s="7" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="J45" s="9" t="s">
         <v>148</v>
@@ -2726,7 +2739,7 @@
         <v>154</v>
       </c>
       <c r="H46" s="6" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="J46" s="9" t="s">
         <v>148</v>
@@ -2746,13 +2759,13 @@
         <v>18</v>
       </c>
       <c r="F47" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="G47" s="7" t="s">
         <v>151</v>
       </c>
       <c r="H47" s="7" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="J47" s="9" t="s">
         <v>148</v>
@@ -2778,10 +2791,10 @@
         <v>154</v>
       </c>
       <c r="H48" s="6" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="I48" s="6" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="J48" t="s">
         <v>148</v>
@@ -2801,13 +2814,13 @@
         <v>18</v>
       </c>
       <c r="F49" s="14" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="G49" s="7" t="s">
         <v>151</v>
       </c>
       <c r="H49" s="7" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="I49" s="8"/>
       <c r="J49" s="9" t="s">
@@ -2834,7 +2847,7 @@
         <v>154</v>
       </c>
       <c r="H50" s="6" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="J50" t="s">
         <v>172</v>
@@ -2854,13 +2867,13 @@
         <v>18</v>
       </c>
       <c r="F51" s="14" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="G51" s="7" t="s">
         <v>151</v>
       </c>
       <c r="H51" s="7" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="I51" s="10"/>
       <c r="J51" s="9" t="s">
@@ -2887,7 +2900,7 @@
         <v>154</v>
       </c>
       <c r="H52" s="6" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="I52" s="6" t="s">
         <v>173</v>
@@ -2910,13 +2923,13 @@
         <v>18</v>
       </c>
       <c r="F53" s="14" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="G53" s="7" t="s">
         <v>151</v>
       </c>
       <c r="H53" s="7" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="I53" s="10"/>
       <c r="J53" s="9" t="s">
@@ -2937,7 +2950,7 @@
         <v>13</v>
       </c>
       <c r="F54" s="14" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G54" s="2" t="s">
         <v>146</v>
@@ -2946,7 +2959,7 @@
         <v>146</v>
       </c>
       <c r="I54" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="J54" s="9" t="s">
         <v>148</v>
@@ -2993,13 +3006,16 @@
         <v>18</v>
       </c>
       <c r="F56" s="14" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="G56" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="H56" s="7" t="s">
-        <v>207</v>
+      <c r="H56" s="21" t="s">
+        <v>205</v>
+      </c>
+      <c r="I56" s="19" t="s">
+        <v>221</v>
       </c>
       <c r="J56" s="2" t="s">
         <v>134</v>
@@ -3048,7 +3064,7 @@
         <v>18</v>
       </c>
       <c r="F58" s="14" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G58" s="2" t="s">
         <v>146</v>
@@ -3083,7 +3099,7 @@
         <v>134</v>
       </c>
       <c r="I59" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="J59" s="2" t="s">
         <v>134</v>
@@ -3112,7 +3128,7 @@
         <v>134</v>
       </c>
       <c r="I60" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="J60" s="2" t="s">
         <v>134</v>

</xml_diff>